<commit_message>
updating excel spreadsheet with latest changes
</commit_message>
<xml_diff>
--- a/Mobile-Friendly-Site-Upgrade-Page-Index.xlsx
+++ b/Mobile-Friendly-Site-Upgrade-Page-Index.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="460" windowWidth="20220" windowHeight="14260" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="3120" yWindow="460" windowWidth="20220" windowHeight="14260" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="All Pages" sheetId="17" r:id="rId1"/>
@@ -4299,11 +4299,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4313,8 +4314,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13123,8 +13125,8 @@
   <dimension ref="A1:G522"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13900,7 +13902,7 @@
       <c r="A66" t="s">
         <v>1396</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>1144</v>
       </c>
       <c r="C66">
@@ -13914,7 +13916,7 @@
       <c r="A67" t="s">
         <v>1396</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="4" t="s">
         <v>1143</v>
       </c>
       <c r="C67">
@@ -13928,7 +13930,7 @@
       <c r="A68" t="s">
         <v>1396</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="4" t="s">
         <v>721</v>
       </c>
       <c r="C68">
@@ -13956,7 +13958,7 @@
       <c r="A70" t="s">
         <v>1396</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="4" t="s">
         <v>719</v>
       </c>
       <c r="C70">
@@ -13970,7 +13972,7 @@
       <c r="A71" t="s">
         <v>1396</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="4" t="s">
         <v>718</v>
       </c>
       <c r="C71">
@@ -13984,7 +13986,7 @@
       <c r="A72" t="s">
         <v>1396</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="4" t="s">
         <v>717</v>
       </c>
       <c r="C72">
@@ -13998,7 +14000,7 @@
       <c r="A73" t="s">
         <v>1396</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="4" t="s">
         <v>716</v>
       </c>
       <c r="C73">
@@ -14012,7 +14014,7 @@
       <c r="A74" t="s">
         <v>1396</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="4" t="s">
         <v>709</v>
       </c>
       <c r="C74">
@@ -14771,7 +14773,7 @@
       <c r="A128" t="s">
         <v>1397</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C128">
@@ -15415,7 +15417,7 @@
       <c r="A174" t="s">
         <v>1397</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="4" t="s">
         <v>171</v>
       </c>
       <c r="C174">

</xml_diff>